<commit_message>
Preparando módulo para migración individual de archivos.
</commit_message>
<xml_diff>
--- a/modulos/data/plantilla_fichas.xlsx
+++ b/modulos/data/plantilla_fichas.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="gFaHzvzhKUF8vyc0azn3eA5wIyuGfo71hHhSuXYfpy0="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="zGFm+uZT7c8Q/9+dQcVcapOkcwc+ZRNqyeU/yfG/2FY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
   <si>
     <t>ci_pasaporte</t>
   </si>
@@ -55,7 +55,7 @@
     <t>fecha_nacimiento</t>
   </si>
   <si>
-    <t>tipo_parroqui</t>
+    <t>tipo_parroquia</t>
   </si>
   <si>
     <t>ciudad</t>
@@ -169,6 +169,9 @@
     <t>tiene_carnet_conadis</t>
   </si>
   <si>
+    <t>codigo_carrera</t>
+  </si>
+  <si>
     <t>Columna</t>
   </si>
   <si>
@@ -211,7 +214,7 @@
     <t>Fecha de nacimiento: (día/mes/año)</t>
   </si>
   <si>
-    <t>Parroquia</t>
+    <t>Parroquia(Urbana, Rural)</t>
   </si>
   <si>
     <t>Ciudad</t>
@@ -320,6 +323,9 @@
   </si>
   <si>
     <t>Tiene el Carnet del CONADIS.</t>
+  </si>
+  <si>
+    <t>Codigo único de la carrera en la que esta matriculado el estudiante</t>
   </si>
 </sst>
 </file>
@@ -399,14 +405,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -643,7 +655,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="50" width="18.88"/>
+    <col customWidth="1" min="1" max="51" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.5" customHeight="1">
@@ -683,7 +695,7 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -794,8 +806,11 @@
       <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AX1" s="4" t="s">
         <v>49</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -821,403 +836,411 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>100</v>
+      <c r="B51" s="7" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>